<commit_message>
carra making one small change to the Python numbering of the excell rows
</commit_message>
<xml_diff>
--- a/GenVeg_params_inputs_1col_TS.xlsx
+++ b/GenVeg_params_inputs_1col_TS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Desktop\Landlab\landlab\notebooks\GenVeg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RDEL1CMC\Desktop\LandLab\landlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5317CB6-B734-43F9-A149-BD3C77EAF040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9996FA69-FB54-44AF-9B7F-FBD429914D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="360" windowWidth="18885" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BIS" sheetId="2" r:id="rId1"/>
@@ -854,20 +854,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" style="20" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="37.44140625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" style="20" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="64.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>37</v>
       </c>
@@ -887,7 +887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -914,7 +914,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -929,7 +929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>92</v>
       </c>
@@ -940,8 +940,11 @@
       <c r="D5" s="21" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="6" t="s">
         <v>19</v>
       </c>
@@ -950,10 +953,10 @@
       <c r="D6" s="22"/>
       <c r="E6" s="2"/>
       <c r="F6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
@@ -965,10 +968,10 @@
         <v>24</v>
       </c>
       <c r="F7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -980,10 +983,10 @@
         <v>45</v>
       </c>
       <c r="F8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
@@ -995,10 +998,10 @@
         <v>305</v>
       </c>
       <c r="F9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1010,10 +1013,10 @@
         <v>228</v>
       </c>
       <c r="F10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="23" t="s">
         <v>69</v>
       </c>
@@ -1027,10 +1030,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="4" t="s">
         <v>46</v>
@@ -1042,10 +1045,10 @@
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="F12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
       <c r="B13" s="4" t="s">
         <v>46</v>
@@ -1057,10 +1060,10 @@
         <v>0.03</v>
       </c>
       <c r="F13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="23" t="s">
         <v>70</v>
       </c>
@@ -1074,10 +1077,10 @@
         <v>1.444</v>
       </c>
       <c r="F14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="4" t="s">
         <v>47</v>
@@ -1089,10 +1092,10 @@
         <v>1.5129999999999999</v>
       </c>
       <c r="F15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="4" t="s">
         <v>47</v>
@@ -1104,10 +1107,10 @@
         <v>1.4630000000000001</v>
       </c>
       <c r="F16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -1119,10 +1122,10 @@
         <v>0.02</v>
       </c>
       <c r="F17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="32.25" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="30.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>89</v>
       </c>
@@ -1134,10 +1137,10 @@
         <v>9</v>
       </c>
       <c r="F18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>11</v>
       </c>
@@ -1149,10 +1152,10 @@
         <v>5.5E-2</v>
       </c>
       <c r="F19">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>20</v>
       </c>
@@ -1161,10 +1164,10 @@
       <c r="D20" s="11"/>
       <c r="E20" s="2"/>
       <c r="F20">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>90</v>
       </c>
@@ -1176,10 +1179,10 @@
         <v>34</v>
       </c>
       <c r="F21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>2</v>
       </c>
@@ -1191,10 +1194,10 @@
         <v>3</v>
       </c>
       <c r="F22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>4</v>
       </c>
@@ -1206,10 +1209,10 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
         <v>3</v>
       </c>
@@ -1221,10 +1224,10 @@
         <v>1.45</v>
       </c>
       <c r="F24">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>82</v>
       </c>
@@ -1238,10 +1241,10 @@
         <v>0.45</v>
       </c>
       <c r="F25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="24"/>
       <c r="B26" s="12" t="s">
         <v>55</v>
@@ -1253,10 +1256,10 @@
         <v>0.3</v>
       </c>
       <c r="F26">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="24"/>
       <c r="B27" s="12" t="s">
         <v>55</v>
@@ -1268,10 +1271,10 @@
         <v>0.25</v>
       </c>
       <c r="F27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16.2" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
         <v>86</v>
       </c>
@@ -1283,10 +1286,10 @@
         <v>0.23100000000000001</v>
       </c>
       <c r="F28">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="24" t="s">
         <v>71</v>
       </c>
@@ -1300,10 +1303,10 @@
         <v>0.01</v>
       </c>
       <c r="F29">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="24"/>
       <c r="B30" s="12" t="s">
         <v>65</v>
@@ -1315,10 +1318,10 @@
         <v>0.1</v>
       </c>
       <c r="F30">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="24"/>
       <c r="B31" s="12" t="s">
         <v>65</v>
@@ -1330,10 +1333,10 @@
         <v>0.5</v>
       </c>
       <c r="F31">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="6" t="s">
         <v>21</v>
       </c>
@@ -1342,10 +1345,10 @@
       <c r="D32" s="11"/>
       <c r="E32" s="2"/>
       <c r="F32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
         <v>9</v>
       </c>
@@ -1357,10 +1360,10 @@
         <v>4</v>
       </c>
       <c r="F33">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -1372,10 +1375,10 @@
         <v>0.5</v>
       </c>
       <c r="F34">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
         <v>22</v>
       </c>
@@ -1387,10 +1390,10 @@
         <v>0</v>
       </c>
       <c r="F35">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="6" t="s">
         <v>31</v>
       </c>
@@ -1399,10 +1402,10 @@
       <c r="D36" s="11"/>
       <c r="E36" s="2"/>
       <c r="F36">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
         <v>32</v>
       </c>
@@ -1414,10 +1417,10 @@
         <v>0.01</v>
       </c>
       <c r="F37">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
         <v>33</v>
       </c>
@@ -1429,10 +1432,10 @@
         <v>365</v>
       </c>
       <c r="F38">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="6" t="s">
         <v>25</v>
       </c>
@@ -1441,10 +1444,10 @@
       <c r="D39" s="11"/>
       <c r="E39" s="2"/>
       <c r="F39">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
         <v>26</v>
       </c>
@@ -1459,10 +1462,10 @@
         <v>28</v>
       </c>
       <c r="F40">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
         <v>27</v>
       </c>
@@ -1474,10 +1477,10 @@
         <v>0.25</v>
       </c>
       <c r="F41">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="6" t="s">
         <v>23</v>
       </c>
@@ -1488,10 +1491,10 @@
         <v>64</v>
       </c>
       <c r="F42">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
         <v>13</v>
       </c>
@@ -1506,10 +1509,10 @@
         <v>36</v>
       </c>
       <c r="F43">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
         <v>15</v>
       </c>
@@ -1521,10 +1524,10 @@
         <v>207</v>
       </c>
       <c r="F44">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
         <v>14</v>
       </c>
@@ -1538,10 +1541,10 @@
         <v>30</v>
       </c>
       <c r="F45">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="12" t="s">
         <v>74</v>
@@ -1553,10 +1556,10 @@
         <v>40</v>
       </c>
       <c r="F46">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="12" t="s">
         <v>74</v>
@@ -1568,10 +1571,10 @@
         <v>50</v>
       </c>
       <c r="F47">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
         <v>29</v>
       </c>
@@ -1585,10 +1588,10 @@
         <v>0.01</v>
       </c>
       <c r="F48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="7"/>
       <c r="B49" s="12" t="s">
         <v>75</v>
@@ -1600,10 +1603,10 @@
         <v>0.25</v>
       </c>
       <c r="F49">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="7"/>
       <c r="B50" s="12" t="s">
         <v>75</v>
@@ -1615,10 +1618,10 @@
         <v>0.67</v>
       </c>
       <c r="F50">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
         <v>87</v>
       </c>
@@ -1632,10 +1635,10 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="7"/>
       <c r="B52" s="12" t="s">
         <v>76</v>
@@ -1647,10 +1650,10 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="7"/>
       <c r="B53" s="12" t="s">
         <v>76</v>
@@ -1662,10 +1665,10 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
         <v>16</v>
       </c>
@@ -1677,10 +1680,10 @@
         <v>35</v>
       </c>
       <c r="F54">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
         <v>18</v>
       </c>
@@ -1692,10 +1695,10 @@
         <v>365</v>
       </c>
       <c r="F55">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
         <v>17</v>
       </c>
@@ -1709,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="F56">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="7"/>
       <c r="B57" s="12" t="s">
         <v>79</v>
@@ -1724,10 +1727,10 @@
         <v>0.2</v>
       </c>
       <c r="F57">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="7"/>
       <c r="B58" s="12" t="s">
         <v>79</v>
@@ -1739,10 +1742,10 @@
         <v>0.5</v>
       </c>
       <c r="F58">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="7"/>
       <c r="B59" s="12" t="s">
         <v>79</v>
@@ -1754,10 +1757,10 @@
         <v>0.68</v>
       </c>
       <c r="F59">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="7"/>
       <c r="B60" s="12" t="s">
         <v>79</v>
@@ -1769,10 +1772,10 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="F60">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
         <v>30</v>
       </c>
@@ -1786,10 +1789,10 @@
         <v>0</v>
       </c>
       <c r="F61">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="7"/>
       <c r="B62" s="12" t="s">
         <v>80</v>
@@ -1801,10 +1804,10 @@
         <v>0</v>
       </c>
       <c r="F62">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="7"/>
       <c r="B63" s="12" t="s">
         <v>80</v>
@@ -1816,10 +1819,10 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="7"/>
       <c r="B64" s="12" t="s">
         <v>80</v>
@@ -1831,10 +1834,10 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="12" t="s">
         <v>80</v>
@@ -1846,10 +1849,10 @@
         <v>1</v>
       </c>
       <c r="F65">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
         <v>88</v>
       </c>
@@ -1863,10 +1866,10 @@
         <v>500</v>
       </c>
       <c r="F66">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="7"/>
       <c r="B67" s="12" t="s">
         <v>81</v>
@@ -1878,10 +1881,10 @@
         <v>300</v>
       </c>
       <c r="F67">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="12" t="s">
         <v>81</v>
@@ -1893,10 +1896,10 @@
         <v>200</v>
       </c>
       <c r="F68">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="7"/>
       <c r="B69" s="12" t="s">
         <v>81</v>
@@ -1908,10 +1911,10 @@
         <v>200</v>
       </c>
       <c r="F69">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="7"/>
       <c r="B70" s="12" t="s">
         <v>81</v>
@@ -1923,660 +1926,660 @@
         <v>300</v>
       </c>
       <c r="F70">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="8"/>
       <c r="B71" s="13"/>
       <c r="C71" s="19"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="8"/>
       <c r="B72" s="13"/>
       <c r="C72" s="19"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="8"/>
       <c r="B73" s="13"/>
       <c r="C73" s="19"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
       <c r="B74" s="13"/>
       <c r="C74" s="19"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="8"/>
       <c r="B75" s="13"/>
       <c r="C75" s="19"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="8"/>
       <c r="B76" s="13"/>
       <c r="C76" s="19"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="8"/>
       <c r="B77" s="13"/>
       <c r="C77" s="19"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="8"/>
       <c r="B78" s="13"/>
       <c r="C78" s="19"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
       <c r="B79" s="13"/>
       <c r="C79" s="19"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
       <c r="B80" s="13"/>
       <c r="C80" s="19"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="8"/>
       <c r="B81" s="13"/>
       <c r="C81" s="19"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="8"/>
       <c r="B82" s="13"/>
       <c r="C82" s="19"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="8"/>
       <c r="B83" s="13"/>
       <c r="C83" s="19"/>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="8"/>
       <c r="B84" s="13"/>
       <c r="C84" s="19"/>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="8"/>
       <c r="B85" s="13"/>
       <c r="C85" s="19"/>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="8"/>
       <c r="B86" s="13"/>
       <c r="C86" s="19"/>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="8"/>
       <c r="B87" s="13"/>
       <c r="C87" s="19"/>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="8"/>
       <c r="B88" s="13"/>
       <c r="C88" s="19"/>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="8"/>
       <c r="B89" s="13"/>
       <c r="C89" s="19"/>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="8"/>
       <c r="B90" s="13"/>
       <c r="C90" s="19"/>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="8"/>
       <c r="B91" s="13"/>
       <c r="C91" s="19"/>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="8"/>
       <c r="B92" s="13"/>
       <c r="C92" s="19"/>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="8"/>
       <c r="B93" s="13"/>
       <c r="C93" s="19"/>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
       <c r="B94" s="13"/>
       <c r="C94" s="19"/>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="8"/>
       <c r="B95" s="13"/>
       <c r="C95" s="19"/>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="8"/>
       <c r="B96" s="13"/>
       <c r="C96" s="19"/>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="8"/>
       <c r="B97" s="13"/>
       <c r="C97" s="19"/>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="8"/>
       <c r="B98" s="13"/>
       <c r="C98" s="19"/>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="8"/>
       <c r="B99" s="13"/>
       <c r="C99" s="19"/>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="8"/>
       <c r="B100" s="13"/>
       <c r="C100" s="19"/>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="8"/>
       <c r="B101" s="13"/>
       <c r="C101" s="19"/>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="8"/>
       <c r="B102" s="13"/>
       <c r="C102" s="19"/>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="8"/>
       <c r="B103" s="13"/>
       <c r="C103" s="19"/>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="8"/>
       <c r="B104" s="13"/>
       <c r="C104" s="19"/>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="8"/>
       <c r="B105" s="13"/>
       <c r="C105" s="19"/>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="8"/>
       <c r="B106" s="13"/>
       <c r="C106" s="19"/>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
       <c r="B107" s="13"/>
       <c r="C107" s="19"/>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="8"/>
       <c r="B108" s="13"/>
       <c r="C108" s="19"/>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="8"/>
       <c r="B109" s="13"/>
       <c r="C109" s="19"/>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="8"/>
       <c r="B110" s="13"/>
       <c r="C110" s="19"/>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="8"/>
       <c r="B111" s="13"/>
       <c r="C111" s="19"/>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="8"/>
       <c r="B112" s="13"/>
       <c r="C112" s="19"/>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="8"/>
       <c r="B113" s="13"/>
       <c r="C113" s="19"/>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="8"/>
       <c r="B114" s="13"/>
       <c r="C114" s="19"/>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="8"/>
       <c r="B115" s="13"/>
       <c r="C115" s="19"/>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="8"/>
       <c r="B116" s="13"/>
       <c r="C116" s="19"/>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="8"/>
       <c r="B117" s="13"/>
       <c r="C117" s="19"/>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="8"/>
       <c r="B118" s="13"/>
       <c r="C118" s="19"/>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="8"/>
       <c r="B119" s="13"/>
       <c r="C119" s="19"/>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="8"/>
       <c r="B120" s="13"/>
       <c r="C120" s="19"/>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="8"/>
       <c r="B121" s="13"/>
       <c r="C121" s="19"/>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="8"/>
       <c r="B122" s="13"/>
       <c r="C122" s="19"/>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="8"/>
       <c r="B123" s="13"/>
       <c r="C123" s="19"/>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="8"/>
       <c r="B124" s="13"/>
       <c r="C124" s="19"/>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="8"/>
       <c r="B125" s="13"/>
       <c r="C125" s="19"/>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="8"/>
       <c r="B126" s="13"/>
       <c r="C126" s="19"/>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="8"/>
       <c r="B127" s="13"/>
       <c r="C127" s="19"/>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
       <c r="B128" s="13"/>
       <c r="C128" s="19"/>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="8"/>
       <c r="B129" s="13"/>
       <c r="C129" s="19"/>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="8"/>
       <c r="B130" s="13"/>
       <c r="C130" s="19"/>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="8"/>
       <c r="B131" s="13"/>
       <c r="C131" s="19"/>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="8"/>
       <c r="B132" s="13"/>
       <c r="C132" s="19"/>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="8"/>
       <c r="B133" s="13"/>
       <c r="C133" s="19"/>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="8"/>
       <c r="B134" s="13"/>
       <c r="C134" s="19"/>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="8"/>
       <c r="B135" s="13"/>
       <c r="C135" s="19"/>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="8"/>
       <c r="B136" s="13"/>
       <c r="C136" s="19"/>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="8"/>
       <c r="B137" s="13"/>
       <c r="C137" s="19"/>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="8"/>
       <c r="B138" s="13"/>
       <c r="C138" s="19"/>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="8"/>
       <c r="B139" s="13"/>
       <c r="C139" s="19"/>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="8"/>
       <c r="B140" s="13"/>
       <c r="C140" s="19"/>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="8"/>
       <c r="B141" s="13"/>
       <c r="C141" s="19"/>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="8"/>
       <c r="B142" s="13"/>
       <c r="C142" s="19"/>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="8"/>
       <c r="B143" s="13"/>
       <c r="C143" s="19"/>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="8"/>
       <c r="B144" s="13"/>
       <c r="C144" s="19"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="8"/>
       <c r="B145" s="13"/>
       <c r="C145" s="19"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="8"/>
       <c r="B146" s="13"/>
       <c r="C146" s="19"/>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="8"/>
       <c r="B147" s="13"/>
       <c r="C147" s="19"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" s="8"/>
       <c r="B148" s="13"/>
       <c r="C148" s="19"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="8"/>
       <c r="B149" s="13"/>
       <c r="C149" s="19"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="8"/>
       <c r="B150" s="13"/>
       <c r="C150" s="19"/>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="8"/>
       <c r="B151" s="13"/>
       <c r="C151" s="19"/>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="8"/>
       <c r="B152" s="13"/>
       <c r="C152" s="19"/>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="8"/>
       <c r="B153" s="13"/>
       <c r="C153" s="19"/>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="8"/>
       <c r="B154" s="13"/>
       <c r="C154" s="19"/>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="8"/>
       <c r="B155" s="13"/>
       <c r="C155" s="19"/>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="8"/>
       <c r="B156" s="13"/>
       <c r="C156" s="19"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="8"/>
       <c r="B157" s="13"/>
       <c r="C157" s="19"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="8"/>
       <c r="B158" s="13"/>
       <c r="C158" s="19"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="8"/>
       <c r="B159" s="13"/>
       <c r="C159" s="19"/>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="8"/>
       <c r="B160" s="13"/>
       <c r="C160" s="19"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" s="8"/>
       <c r="B161" s="13"/>
       <c r="C161" s="19"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" s="8"/>
       <c r="B162" s="13"/>
       <c r="C162" s="19"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" s="8"/>
       <c r="B163" s="13"/>
       <c r="C163" s="19"/>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
       <c r="B164" s="13"/>
       <c r="C164" s="19"/>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" s="8"/>
       <c r="B165" s="13"/>
       <c r="C165" s="19"/>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" s="8"/>
       <c r="B166" s="13"/>
       <c r="C166" s="19"/>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" s="8"/>
       <c r="B167" s="13"/>
       <c r="C167" s="19"/>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" s="8"/>
       <c r="B168" s="13"/>
       <c r="C168" s="19"/>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" s="8"/>
       <c r="B169" s="13"/>
       <c r="C169" s="19"/>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" s="8"/>
       <c r="B170" s="13"/>
       <c r="C170" s="19"/>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" s="8"/>
       <c r="B171" s="13"/>
       <c r="C171" s="19"/>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" s="8"/>
       <c r="B172" s="13"/>
       <c r="C172" s="19"/>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" s="8"/>
       <c r="B173" s="13"/>
       <c r="C173" s="19"/>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" s="8"/>
       <c r="B174" s="13"/>
       <c r="C174" s="19"/>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" s="8"/>
       <c r="B175" s="13"/>
       <c r="C175" s="19"/>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" s="8"/>
       <c r="B176" s="13"/>
       <c r="C176" s="19"/>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" s="8"/>
       <c r="B177" s="13"/>
       <c r="C177" s="19"/>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" s="8"/>
       <c r="B178" s="13"/>
       <c r="C178" s="19"/>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" s="8"/>
       <c r="B179" s="13"/>
       <c r="C179" s="19"/>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" s="8"/>
       <c r="B180" s="13"/>
       <c r="C180" s="19"/>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" s="8"/>
       <c r="B181" s="13"/>
       <c r="C181" s="19"/>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" s="8"/>
       <c r="B182" s="13"/>
       <c r="C182" s="19"/>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" s="8"/>
       <c r="B183" s="13"/>
       <c r="C183" s="19"/>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" s="8"/>
       <c r="B184" s="13"/>
       <c r="C184" s="19"/>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" s="8"/>
       <c r="B185" s="13"/>
       <c r="C185" s="19"/>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" s="8"/>
       <c r="B186" s="13"/>
       <c r="C186" s="19"/>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" s="8"/>
       <c r="B187" s="13"/>
       <c r="C187" s="19"/>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" s="8"/>
       <c r="B188" s="13"/>
       <c r="C188" s="19"/>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" s="8"/>
       <c r="B189" s="13"/>
       <c r="C189" s="19"/>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" s="8"/>
       <c r="B190" s="13"/>
       <c r="C190" s="19"/>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" s="8"/>
       <c r="B191" s="13"/>
       <c r="C191" s="19"/>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" s="8"/>
       <c r="B192" s="13"/>
       <c r="C192" s="19"/>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" s="8"/>
       <c r="B193" s="13"/>
       <c r="C193" s="19"/>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" s="8"/>
       <c r="B194" s="13"/>
       <c r="C194" s="19"/>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" s="8"/>
       <c r="B195" s="13"/>
       <c r="C195" s="19"/>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" s="8"/>
       <c r="B196" s="13"/>
       <c r="C196" s="19"/>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" s="8"/>
       <c r="B197" s="13"/>
       <c r="C197" s="19"/>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" s="8"/>
       <c r="B198" s="13"/>
       <c r="C198" s="19"/>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" s="8"/>
       <c r="B199" s="13"/>
       <c r="C199" s="19"/>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" s="8"/>
       <c r="B200" s="13"/>
       <c r="C200" s="19"/>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" s="8"/>
       <c r="B201" s="13"/>
       <c r="C201" s="19"/>

</xml_diff>